<commit_message>
Tweaks to AV rating curve and separate code for Q
Added another script to just look at Q. Wrote a quickie for doing Q from
a single AV measurment
</commit_message>
<xml_diff>
--- a/Data/Q/Discharge Location Descriptions-compare with Mannings.xlsx
+++ b/Data/Q/Discharge Location Descriptions-compare with Mannings.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\Fagaalu-Sediment-Flux\Data\Q\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7965" activeTab="3"/>
   </bookViews>
@@ -12,7 +17,7 @@
     <sheet name="LBJ" sheetId="3" r:id="rId3"/>
     <sheet name="LBJ-mannings" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -217,13 +222,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.00000"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="00.00"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="00.00"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -463,7 +470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -513,27 +520,47 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -561,10 +588,12 @@
       </c:layout>
       <c:overlay val="1"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -679,40 +708,58 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="87715200"/>
-        <c:axId val="87896832"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="252828912"/>
+        <c:axId val="252828520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="87715200"/>
+        <c:axId val="252828912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87896832"/>
+        <c:crossAx val="252828520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87896832"/>
+        <c:axId val="252828520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87715200"/>
+        <c:crossAx val="252828912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -724,12 +771,24 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -802,40 +861,58 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="88086016"/>
-        <c:axId val="88087552"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="252827344"/>
+        <c:axId val="252827736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="88086016"/>
+        <c:axId val="252827344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88087552"/>
+        <c:crossAx val="252827736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88087552"/>
+        <c:axId val="252827736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88086016"/>
+        <c:crossAx val="252827344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -847,7 +924,17 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -880,6 +967,7 @@
       </c:layout>
       <c:overlay val="1"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -894,6 +982,7 @@
       </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -996,16 +1085,26 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="88164608"/>
-        <c:axId val="88170880"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="252829696"/>
+        <c:axId val="252830088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="88164608"/>
+        <c:axId val="252829696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1024,20 +1123,25 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88170880"/>
+        <c:crossAx val="252830088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88170880"/>
+        <c:axId val="252830088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -1057,15 +1161,20 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88164608"/>
+        <c:crossAx val="252829696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1268,7 +1377,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1300,9 +1409,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1334,6 +1444,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1509,20 +1620,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.85546875" customWidth="1"/>
     <col min="11" max="11" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1539,7 +1650,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="15.75" thickBot="1">
+    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -1553,7 +1664,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1568,7 +1679,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="9"/>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
@@ -1597,7 +1708,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="14">
         <v>0</v>
       </c>
@@ -1629,7 +1740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="14">
         <v>0.5</v>
       </c>
@@ -1664,7 +1775,7 @@
         <v>2.5069799999999998E-3</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="14">
         <v>1</v>
       </c>
@@ -1699,7 +1810,7 @@
         <v>6.4007999999999999E-3</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="14">
         <v>1.5</v>
       </c>
@@ -1734,7 +1845,7 @@
         <v>7.4675999999999996E-3</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="14">
         <v>2</v>
       </c>
@@ -1769,7 +1880,7 @@
         <v>8.32104E-3</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="14">
         <v>2.5</v>
       </c>
@@ -1804,7 +1915,7 @@
         <v>7.0408799999999994E-3</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="14">
         <v>3</v>
       </c>
@@ -1839,7 +1950,7 @@
         <v>7.498079999999999E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:10">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="14">
         <v>3.5</v>
       </c>
@@ -1874,7 +1985,7 @@
         <v>6.7894200000000009E-3</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="14">
         <v>4</v>
       </c>
@@ -1909,7 +2020,7 @@
         <v>4.6939199999999999E-3</v>
       </c>
     </row>
-    <row r="15" spans="2:10">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="14">
         <v>4.5</v>
       </c>
@@ -1944,7 +2055,7 @@
         <v>4.0843199999999998E-3</v>
       </c>
     </row>
-    <row r="16" spans="2:10">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="14">
         <v>5</v>
       </c>
@@ -1979,7 +2090,7 @@
         <v>2.1336000000000003E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:14">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="14">
         <v>5.5</v>
       </c>
@@ -2014,7 +2125,7 @@
         <v>1.0363200000000001E-3</v>
       </c>
     </row>
-    <row r="18" spans="2:14">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="14">
         <v>6</v>
       </c>
@@ -2049,7 +2160,7 @@
         <v>3.2004000000000001E-4</v>
       </c>
     </row>
-    <row r="19" spans="2:14">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="14">
         <v>6.5</v>
       </c>
@@ -2084,7 +2195,7 @@
         <v>6.0959999999999996E-4</v>
       </c>
     </row>
-    <row r="20" spans="2:14" ht="15.75" thickBot="1">
+    <row r="20" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="18">
         <v>7</v>
       </c>
@@ -2119,7 +2230,7 @@
         <v>1.5697200000000001E-3</v>
       </c>
     </row>
-    <row r="21" spans="2:14">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C21">
         <f>AVERAGE(C7:C20)</f>
         <v>5.3571428571428568</v>
@@ -2148,7 +2259,7 @@
         <v>58.902600000000007</v>
       </c>
     </row>
-    <row r="22" spans="2:14">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H22" t="s">
         <v>17</v>
       </c>
@@ -2164,20 +2275,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" activeCellId="1" sqref="A5:A12 D5:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2194,7 +2305,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1">
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -2208,7 +2319,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -2223,7 +2334,7 @@
       <c r="H3" s="8"/>
       <c r="I3" s="9"/>
     </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1">
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>8</v>
       </c>
@@ -2252,7 +2363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="24">
         <v>0</v>
       </c>
@@ -2284,7 +2395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>1</v>
       </c>
@@ -2319,7 +2430,7 @@
         <v>7.0104E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>2</v>
       </c>
@@ -2354,7 +2465,7 @@
         <v>2.033016E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <v>3</v>
       </c>
@@ -2389,7 +2500,7 @@
         <v>2.6289E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>4</v>
       </c>
@@ -2424,7 +2535,7 @@
         <v>3.4564319999999996E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>5</v>
       </c>
@@ -2459,7 +2570,7 @@
         <v>2.6944320000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <v>6</v>
       </c>
@@ -2494,7 +2605,7 @@
         <v>1.9339560000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15.75" thickBot="1">
+    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18">
         <v>7</v>
       </c>
@@ -2528,7 +2639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G13" t="s">
         <v>16</v>
       </c>
@@ -2553,7 +2664,7 @@
         <v>134.47775999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G14" t="s">
         <v>17</v>
       </c>
@@ -2569,14 +2680,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" style="30" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="30" customWidth="1"/>
@@ -2590,7 +2701,7 @@
     <col min="13" max="16384" width="9.140625" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
@@ -2607,7 +2718,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1">
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
         <v>19</v>
       </c>
@@ -2624,7 +2735,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>6</v>
       </c>
@@ -2642,7 +2753,7 @@
       <c r="K3" s="34"/>
       <c r="L3" s="35"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
         <v>8</v>
       </c>
@@ -2680,7 +2791,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="40">
         <v>0</v>
       </c>
@@ -2724,7 +2835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="40">
         <v>1</v>
       </c>
@@ -2771,7 +2882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="40">
         <v>2</v>
       </c>
@@ -2818,7 +2929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="40">
         <v>2.5</v>
       </c>
@@ -2865,7 +2976,7 @@
         <v>8.2295999999999986E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="40">
         <v>3</v>
       </c>
@@ -2912,7 +3023,7 @@
         <v>1.0027920000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="40">
         <v>3.5</v>
       </c>
@@ -2959,7 +3070,7 @@
         <v>1.016508E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="40">
         <v>4</v>
       </c>
@@ -3006,7 +3117,7 @@
         <v>1.0287000000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="40">
         <v>4.5</v>
       </c>
@@ -3053,7 +3164,7 @@
         <v>3.0723839999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="40">
         <v>5</v>
       </c>
@@ -3100,7 +3211,7 @@
         <v>3.4137599999999997E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="40">
         <v>5.5</v>
       </c>
@@ -3147,7 +3258,7 @@
         <v>1.0607039999999998E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="40">
         <v>6</v>
       </c>
@@ -3194,7 +3305,7 @@
         <v>1.9659600000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="40">
         <v>6.5</v>
       </c>
@@ -3241,7 +3352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15.75" thickBot="1">
+    <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="43">
         <v>7</v>
       </c>
@@ -3288,7 +3399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J18" s="30" t="s">
         <v>16</v>
       </c>
@@ -3297,7 +3408,7 @@
         <v>0.10873740000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J19" s="30" t="s">
         <v>17</v>
       </c>
@@ -3306,17 +3417,17 @@
         <v>108.73740000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B21" s="30" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22" s="30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="30" t="s">
         <v>30</v>
       </c>
@@ -3331,7 +3442,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B24" s="30" t="s">
         <v>24</v>
       </c>
@@ -3343,7 +3454,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B25" s="30" t="s">
         <v>26</v>
       </c>
@@ -3361,7 +3472,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B26" s="30" t="s">
         <v>23</v>
       </c>
@@ -3378,7 +3489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B27" s="30" t="s">
         <v>22</v>
       </c>
@@ -3393,12 +3504,12 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C28" s="30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" s="30" t="s">
         <v>36</v>
       </c>
@@ -3410,7 +3521,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B30" s="30" t="s">
         <v>39</v>
       </c>
@@ -3422,7 +3533,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C31" s="46">
         <f>C30*1000</f>
         <v>310.52287607009805</v>
@@ -3439,15 +3550,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AD34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="U23" sqref="U23:W41"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
@@ -3463,15 +3575,16 @@
     <col min="16" max="16" width="16.28515625" customWidth="1"/>
     <col min="17" max="17" width="16" customWidth="1"/>
     <col min="19" max="19" width="12.5703125" customWidth="1"/>
+    <col min="21" max="21" width="16.42578125" customWidth="1"/>
     <col min="28" max="28" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:30" ht="15.75" thickBot="1">
+    <row r="1" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="2:30">
+    <row r="2" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
@@ -3501,7 +3614,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="2:30">
+    <row r="3" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B3" s="21" t="s">
         <v>8</v>
       </c>
@@ -3581,7 +3694,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="2:30">
+    <row r="4" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B4" s="14">
         <v>0</v>
       </c>
@@ -3625,7 +3738,7 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <f>(C4+C5)/2</f>
+        <f t="shared" ref="N4:N19" si="1">(C4+C5)/2</f>
         <v>3</v>
       </c>
       <c r="O4">
@@ -3674,7 +3787,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="5" spans="2:30">
+    <row r="5" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B5" s="14">
         <v>1</v>
       </c>
@@ -3685,7 +3798,7 @@
         <v>0.39</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E20" si="1">0-C5</f>
+        <f t="shared" ref="E5:E20" si="2">0-C5</f>
         <v>-6</v>
       </c>
       <c r="F5">
@@ -3696,15 +3809,15 @@
         <f>F5*2.54</f>
         <v>30.48</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="58">
         <f>C5*G5</f>
         <v>182.88</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="59">
         <f>H5/10000</f>
         <v>1.8287999999999999E-2</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="59">
         <f t="shared" si="0"/>
         <v>7.1323200000000002E-3</v>
       </c>
@@ -3721,7 +3834,7 @@
         <v>3</v>
       </c>
       <c r="N5">
-        <f>(C5+C6)/2</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="O5">
@@ -3740,7 +3853,7 @@
         <v>1.9812E-2</v>
       </c>
       <c r="S5">
-        <f t="shared" ref="S5:S20" si="2">R5*D5</f>
+        <f t="shared" ref="S5:S20" si="3">R5*D5</f>
         <v>7.7266800000000005E-3</v>
       </c>
       <c r="U5">
@@ -3774,7 +3887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:30">
+    <row r="6" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B6" s="14">
         <v>2</v>
       </c>
@@ -3785,62 +3898,62 @@
         <v>0.25</v>
       </c>
       <c r="E6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-14</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F20" si="3">(B6-B5)*12</f>
+        <f t="shared" ref="F6:F20" si="4">(B6-B5)*12</f>
         <v>12</v>
       </c>
       <c r="G6">
-        <f t="shared" ref="G6:G20" si="4">F6*2.54</f>
-        <v>30.48</v>
-      </c>
-      <c r="H6">
-        <f t="shared" ref="H6:H20" si="5">C6*G6</f>
+        <f t="shared" ref="G6:G20" si="5">F6*2.54</f>
+        <v>30.48</v>
+      </c>
+      <c r="H6" s="58">
+        <f t="shared" ref="H6:H20" si="6">C6*G6</f>
         <v>426.72</v>
       </c>
-      <c r="I6">
-        <f t="shared" ref="I6:I20" si="6">H6/10000</f>
+      <c r="I6" s="59">
+        <f t="shared" ref="I6:I20" si="7">H6/10000</f>
         <v>4.2672000000000002E-2</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="59">
         <f t="shared" si="0"/>
         <v>1.0668E-2</v>
       </c>
       <c r="K6">
-        <f t="shared" ref="K6:K20" si="7">B6</f>
+        <f t="shared" ref="K6:K20" si="8">B6</f>
         <v>2</v>
       </c>
       <c r="L6">
-        <f t="shared" ref="L6:L20" si="8">L5+1</f>
+        <f t="shared" ref="L6:L20" si="9">L5+1</f>
         <v>2.5</v>
       </c>
       <c r="M6">
-        <f t="shared" ref="M6:M20" si="9">N5</f>
+        <f t="shared" ref="M6:M20" si="10">N5</f>
         <v>10</v>
       </c>
       <c r="N6">
-        <f>(C6+C7)/2</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="O6">
         <v>30.48</v>
       </c>
       <c r="P6" s="56">
-        <f>SQRT((C6-C5)^2+((B6-B5)*12*2.54)^2)</f>
+        <f t="shared" ref="P5:P20" si="11">SQRT((C6-C5)^2+((B6-B5)*12*2.54)^2)</f>
         <v>31.512384866905901</v>
       </c>
       <c r="Q6">
-        <f t="shared" ref="Q6:Q20" si="10">1/2*(M6+N6)*O6</f>
+        <f t="shared" ref="Q6:Q20" si="12">1/2*(M6+N6)*O6</f>
         <v>365.76</v>
       </c>
       <c r="R6">
-        <f t="shared" ref="R5:R20" si="11">Q6/10000</f>
+        <f t="shared" ref="R6:R20" si="13">Q6/10000</f>
         <v>3.6575999999999997E-2</v>
       </c>
       <c r="S6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.1439999999999994E-3</v>
       </c>
       <c r="U6">
@@ -3874,7 +3987,7 @@
         <v>0.31064900000000001</v>
       </c>
     </row>
-    <row r="7" spans="2:30">
+    <row r="7" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B7" s="14">
         <v>3</v>
       </c>
@@ -3885,62 +3998,62 @@
         <v>0.24</v>
       </c>
       <c r="E7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-14</v>
       </c>
       <c r="F7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="G7">
-        <f t="shared" si="4"/>
-        <v>30.48</v>
-      </c>
-      <c r="H7">
         <f t="shared" si="5"/>
+        <v>30.48</v>
+      </c>
+      <c r="H7" s="58">
+        <f t="shared" si="6"/>
         <v>426.72</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="6"/>
+      <c r="I7" s="59">
+        <f t="shared" si="7"/>
         <v>4.2672000000000002E-2</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="59">
         <f t="shared" si="0"/>
         <v>1.024128E-2</v>
       </c>
       <c r="K7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="L7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3.5</v>
       </c>
       <c r="M7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>14</v>
       </c>
       <c r="N7">
-        <f>(C7+C8)/2</f>
+        <f t="shared" si="1"/>
         <v>16.5</v>
       </c>
       <c r="O7">
         <v>30.48</v>
       </c>
       <c r="P7" s="56">
-        <f>SQRT((C7-C6)^2+((B7-B6)*12*2.54)^2)</f>
+        <f t="shared" si="11"/>
         <v>30.48</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>464.82</v>
       </c>
       <c r="R7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>4.6482000000000002E-2</v>
       </c>
       <c r="S7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1155679999999999E-2</v>
       </c>
       <c r="U7">
@@ -3974,7 +4087,7 @@
         <v>0.31512400000000002</v>
       </c>
     </row>
-    <row r="8" spans="2:30">
+    <row r="8" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B8" s="14">
         <v>4</v>
       </c>
@@ -3985,1261 +4098,1261 @@
         <v>0.06</v>
       </c>
       <c r="E8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-19</v>
       </c>
       <c r="F8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="G8">
-        <f t="shared" si="4"/>
-        <v>30.48</v>
-      </c>
-      <c r="H8">
         <f t="shared" si="5"/>
+        <v>30.48</v>
+      </c>
+      <c r="H8" s="58">
+        <f t="shared" si="6"/>
         <v>579.12</v>
       </c>
-      <c r="I8">
-        <f t="shared" si="6"/>
+      <c r="I8" s="59">
+        <f t="shared" si="7"/>
         <v>5.7911999999999998E-2</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="59">
         <f t="shared" si="0"/>
         <v>3.4747199999999997E-3</v>
       </c>
       <c r="K8">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="9"/>
+        <v>4.5</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="10"/>
+        <v>16.5</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="1"/>
+        <v>19.5</v>
+      </c>
+      <c r="O8">
+        <v>30.48</v>
+      </c>
+      <c r="P8" s="56">
+        <f t="shared" si="11"/>
+        <v>30.887382537210886</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="12"/>
+        <v>548.64</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="13"/>
+        <v>5.4863999999999996E-2</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="3"/>
+        <v>3.2918399999999994E-3</v>
+      </c>
+      <c r="U8">
+        <v>3</v>
+      </c>
+      <c r="V8">
+        <v>3</v>
+      </c>
+      <c r="W8">
+        <v>14</v>
+      </c>
+      <c r="X8">
+        <v>0.24</v>
+      </c>
+      <c r="Y8">
+        <v>30.48</v>
+      </c>
+      <c r="Z8">
+        <v>14</v>
+      </c>
+      <c r="AA8">
+        <v>16.5</v>
+      </c>
+      <c r="AB8">
+        <v>4.6482000000000002E-2</v>
+      </c>
+      <c r="AC8">
+        <v>11.15568</v>
+      </c>
+      <c r="AD8">
+        <v>0.30480000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B9" s="14">
+        <v>5</v>
+      </c>
+      <c r="C9" s="15">
+        <v>20</v>
+      </c>
+      <c r="D9" s="16">
+        <v>0.32</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>-20</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="5"/>
+        <v>30.48</v>
+      </c>
+      <c r="H9" s="58">
+        <f t="shared" si="6"/>
+        <v>609.6</v>
+      </c>
+      <c r="I9" s="59">
         <f t="shared" si="7"/>
+        <v>6.096E-2</v>
+      </c>
+      <c r="J9" s="59">
+        <f t="shared" si="0"/>
+        <v>1.9507199999999999E-2</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="9"/>
+        <v>5.5</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="10"/>
+        <v>19.5</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="O9">
+        <v>30.48</v>
+      </c>
+      <c r="P9" s="56">
+        <f t="shared" si="11"/>
+        <v>30.496399787515902</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="12"/>
+        <v>541.02</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="13"/>
+        <v>5.4101999999999997E-2</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="3"/>
+        <v>1.7312640000000001E-2</v>
+      </c>
+      <c r="U9">
         <v>4</v>
       </c>
-      <c r="L8">
+      <c r="V9">
+        <v>4</v>
+      </c>
+      <c r="W9">
+        <v>19</v>
+      </c>
+      <c r="X9">
+        <v>0.06</v>
+      </c>
+      <c r="Y9">
+        <v>30.48</v>
+      </c>
+      <c r="Z9">
+        <v>16.5</v>
+      </c>
+      <c r="AA9">
+        <v>19.5</v>
+      </c>
+      <c r="AB9">
+        <v>5.4864000000000003E-2</v>
+      </c>
+      <c r="AC9">
+        <v>3.2918400000000001</v>
+      </c>
+      <c r="AD9">
+        <v>0.30887399999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B10" s="14">
+        <v>6</v>
+      </c>
+      <c r="C10" s="15">
+        <v>12</v>
+      </c>
+      <c r="D10" s="16">
+        <v>0.47</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>-12</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="5"/>
+        <v>30.48</v>
+      </c>
+      <c r="H10" s="58">
+        <f t="shared" si="6"/>
+        <v>365.76</v>
+      </c>
+      <c r="I10" s="59">
+        <f t="shared" si="7"/>
+        <v>3.6575999999999997E-2</v>
+      </c>
+      <c r="J10" s="59">
+        <f t="shared" si="0"/>
+        <v>1.7190719999999996E-2</v>
+      </c>
+      <c r="K10">
         <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="9"/>
+        <v>6.5</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="10"/>
+        <v>16</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="O10">
+        <v>30.48</v>
+      </c>
+      <c r="P10" s="56">
+        <f t="shared" si="11"/>
+        <v>31.512384866905901</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="12"/>
+        <v>411.48</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="13"/>
+        <v>4.1148000000000004E-2</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="3"/>
+        <v>1.9339560000000002E-2</v>
+      </c>
+      <c r="U10">
+        <v>5</v>
+      </c>
+      <c r="V10">
+        <v>5</v>
+      </c>
+      <c r="W10">
+        <v>20</v>
+      </c>
+      <c r="X10">
+        <v>0.32</v>
+      </c>
+      <c r="Y10">
+        <v>30.48</v>
+      </c>
+      <c r="Z10">
+        <v>19.5</v>
+      </c>
+      <c r="AA10">
+        <v>16</v>
+      </c>
+      <c r="AB10">
+        <v>5.4101999999999997E-2</v>
+      </c>
+      <c r="AC10">
+        <v>17.312639999999998</v>
+      </c>
+      <c r="AD10">
+        <v>0.30496400000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B11" s="14">
+        <v>7</v>
+      </c>
+      <c r="C11" s="15">
+        <v>10</v>
+      </c>
+      <c r="D11" s="16">
+        <v>0.26</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>-10</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="5"/>
+        <v>30.48</v>
+      </c>
+      <c r="H11" s="58">
+        <f t="shared" si="6"/>
+        <v>304.8</v>
+      </c>
+      <c r="I11" s="59">
+        <f t="shared" si="7"/>
+        <v>3.048E-2</v>
+      </c>
+      <c r="J11" s="59">
+        <f t="shared" si="0"/>
+        <v>7.9248000000000009E-3</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="9"/>
+        <v>7.5</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="10"/>
+        <v>11</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="O11">
+        <v>30.48</v>
+      </c>
+      <c r="P11" s="56">
+        <f t="shared" si="11"/>
+        <v>30.545546320208452</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="12"/>
+        <v>320.04000000000002</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="13"/>
+        <v>3.2004000000000005E-2</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="3"/>
+        <v>8.3210400000000018E-3</v>
+      </c>
+      <c r="U11">
+        <v>6</v>
+      </c>
+      <c r="V11">
+        <v>6</v>
+      </c>
+      <c r="W11">
+        <v>12</v>
+      </c>
+      <c r="X11">
+        <v>0.47</v>
+      </c>
+      <c r="Y11">
+        <v>30.48</v>
+      </c>
+      <c r="Z11">
+        <v>16</v>
+      </c>
+      <c r="AA11">
+        <v>11</v>
+      </c>
+      <c r="AB11">
+        <v>4.1147999999999997E-2</v>
+      </c>
+      <c r="AC11">
+        <v>19.339559999999999</v>
+      </c>
+      <c r="AD11">
+        <v>0.31512400000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B12" s="14">
+        <v>8</v>
+      </c>
+      <c r="C12" s="15">
+        <v>10</v>
+      </c>
+      <c r="D12" s="16">
+        <v>0.33</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>-10</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="5"/>
+        <v>30.48</v>
+      </c>
+      <c r="H12" s="58">
+        <f t="shared" si="6"/>
+        <v>304.8</v>
+      </c>
+      <c r="I12" s="59">
+        <f t="shared" si="7"/>
+        <v>3.048E-2</v>
+      </c>
+      <c r="J12" s="59">
+        <f t="shared" si="0"/>
+        <v>1.00584E-2</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="9"/>
+        <v>8.5</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="O12">
+        <v>30.48</v>
+      </c>
+      <c r="P12" s="56">
+        <f t="shared" si="11"/>
+        <v>30.48</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="12"/>
+        <v>259.08</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="13"/>
+        <v>2.5907999999999997E-2</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="3"/>
+        <v>8.549639999999999E-3</v>
+      </c>
+      <c r="U12">
+        <v>7</v>
+      </c>
+      <c r="V12">
+        <v>7</v>
+      </c>
+      <c r="W12">
+        <v>10</v>
+      </c>
+      <c r="X12">
+        <v>0.26</v>
+      </c>
+      <c r="Y12">
+        <v>30.48</v>
+      </c>
+      <c r="Z12">
+        <v>11</v>
+      </c>
+      <c r="AA12">
+        <v>10</v>
+      </c>
+      <c r="AB12">
+        <v>3.2003999999999998E-2</v>
+      </c>
+      <c r="AC12">
+        <v>8.32104</v>
+      </c>
+      <c r="AD12">
+        <v>0.30545499999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B13" s="14">
+        <v>9</v>
+      </c>
+      <c r="C13" s="15">
+        <v>4</v>
+      </c>
+      <c r="D13" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>-4</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="5"/>
+        <v>30.48</v>
+      </c>
+      <c r="H13" s="58">
+        <f t="shared" si="6"/>
+        <v>121.92</v>
+      </c>
+      <c r="I13" s="59">
+        <f t="shared" si="7"/>
+        <v>1.2192E-2</v>
+      </c>
+      <c r="J13" s="59">
+        <f t="shared" si="0"/>
+        <v>2.4384000000000003E-3</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="9"/>
+        <v>9.5</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="10"/>
+        <v>7</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="O13">
+        <v>30.48</v>
+      </c>
+      <c r="P13" s="56">
+        <f t="shared" si="11"/>
+        <v>31.064938435477384</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="12"/>
+        <v>198.12</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="13"/>
+        <v>1.9812E-2</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="3"/>
+        <v>3.9624000000000005E-3</v>
+      </c>
+      <c r="U13">
+        <v>8</v>
+      </c>
+      <c r="V13">
+        <v>8</v>
+      </c>
+      <c r="W13">
+        <v>10</v>
+      </c>
+      <c r="X13">
+        <v>0.33</v>
+      </c>
+      <c r="Y13">
+        <v>30.48</v>
+      </c>
+      <c r="Z13">
+        <v>10</v>
+      </c>
+      <c r="AA13">
+        <v>7</v>
+      </c>
+      <c r="AB13">
+        <v>2.5908E-2</v>
+      </c>
+      <c r="AC13">
+        <v>8.5496400000000001</v>
+      </c>
+      <c r="AD13">
+        <v>0.30480000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B14" s="14">
+        <v>10</v>
+      </c>
+      <c r="C14" s="15">
+        <v>8</v>
+      </c>
+      <c r="D14" s="16">
+        <v>0.13</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>-8</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="5"/>
+        <v>30.48</v>
+      </c>
+      <c r="H14" s="58">
+        <f t="shared" si="6"/>
+        <v>243.84</v>
+      </c>
+      <c r="I14" s="59">
+        <f t="shared" si="7"/>
+        <v>2.4383999999999999E-2</v>
+      </c>
+      <c r="J14" s="59">
+        <f t="shared" si="0"/>
+        <v>3.1699200000000001E-3</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="9"/>
+        <v>10.5</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+      <c r="O14">
+        <v>30.48</v>
+      </c>
+      <c r="P14" s="56">
+        <f t="shared" si="11"/>
+        <v>30.741346749939243</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="12"/>
+        <v>205.74</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="13"/>
+        <v>2.0574000000000002E-2</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="3"/>
+        <v>2.6746200000000004E-3</v>
+      </c>
+      <c r="U14">
+        <v>9</v>
+      </c>
+      <c r="V14">
+        <v>9</v>
+      </c>
+      <c r="W14">
+        <v>4</v>
+      </c>
+      <c r="X14">
+        <v>0.2</v>
+      </c>
+      <c r="Y14">
+        <v>30.48</v>
+      </c>
+      <c r="Z14">
+        <v>7</v>
+      </c>
+      <c r="AA14">
+        <v>6</v>
+      </c>
+      <c r="AB14">
+        <v>1.9812E-2</v>
+      </c>
+      <c r="AC14">
+        <v>3.9624000000000001</v>
+      </c>
+      <c r="AD14">
+        <v>0.31064900000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B15" s="14">
+        <v>11</v>
+      </c>
+      <c r="C15" s="15">
+        <v>7</v>
+      </c>
+      <c r="D15" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>-7</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="5"/>
+        <v>30.48</v>
+      </c>
+      <c r="H15" s="58">
+        <f t="shared" si="6"/>
+        <v>213.36</v>
+      </c>
+      <c r="I15" s="59">
+        <f t="shared" si="7"/>
+        <v>2.1336000000000001E-2</v>
+      </c>
+      <c r="J15" s="59">
+        <f t="shared" si="0"/>
+        <v>4.2672000000000001E-4</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="9"/>
+        <v>11.5</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="10"/>
+        <v>7.5</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-      <c r="M8">
+      <c r="O15">
+        <v>30.48</v>
+      </c>
+      <c r="P15" s="56">
+        <f t="shared" si="11"/>
+        <v>30.496399787515902</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="12"/>
+        <v>182.88</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="13"/>
+        <v>1.8287999999999999E-2</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="3"/>
+        <v>3.6575999999999997E-4</v>
+      </c>
+      <c r="U15">
+        <v>10</v>
+      </c>
+      <c r="V15">
+        <v>10</v>
+      </c>
+      <c r="W15">
+        <v>8</v>
+      </c>
+      <c r="X15">
+        <v>0.13</v>
+      </c>
+      <c r="Y15">
+        <v>30.48</v>
+      </c>
+      <c r="Z15">
+        <v>6</v>
+      </c>
+      <c r="AA15">
+        <v>7.5</v>
+      </c>
+      <c r="AB15">
+        <v>2.0573999999999999E-2</v>
+      </c>
+      <c r="AC15">
+        <v>2.67462</v>
+      </c>
+      <c r="AD15">
+        <v>0.30741299999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B16" s="14">
+        <v>12</v>
+      </c>
+      <c r="C16" s="15">
+        <v>2</v>
+      </c>
+      <c r="D16" s="16">
+        <v>0.45</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="5"/>
+        <v>30.48</v>
+      </c>
+      <c r="H16" s="58">
+        <f t="shared" si="6"/>
+        <v>60.96</v>
+      </c>
+      <c r="I16" s="59">
+        <f t="shared" si="7"/>
+        <v>6.0959999999999999E-3</v>
+      </c>
+      <c r="J16" s="59">
+        <f t="shared" si="0"/>
+        <v>2.7431999999999999E-3</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="9"/>
+        <v>12.5</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="10"/>
+        <v>4.5</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+      <c r="O16">
+        <v>30.48</v>
+      </c>
+      <c r="P16" s="56">
+        <f t="shared" si="11"/>
+        <v>30.887382537210886</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="12"/>
+        <v>121.92</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="13"/>
+        <v>1.2192E-2</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="3"/>
+        <v>5.4863999999999998E-3</v>
+      </c>
+      <c r="U16">
+        <v>11</v>
+      </c>
+      <c r="V16">
+        <v>11</v>
+      </c>
+      <c r="W16">
+        <v>7</v>
+      </c>
+      <c r="X16">
+        <v>0.02</v>
+      </c>
+      <c r="Y16">
+        <v>30.48</v>
+      </c>
+      <c r="Z16">
+        <v>7.5</v>
+      </c>
+      <c r="AA16">
+        <v>4.5</v>
+      </c>
+      <c r="AB16">
+        <v>1.8287999999999999E-2</v>
+      </c>
+      <c r="AC16">
+        <v>0.36575999999999997</v>
+      </c>
+      <c r="AD16">
+        <v>0.30496400000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B17" s="50">
+        <v>13</v>
+      </c>
+      <c r="C17" s="17">
+        <v>5</v>
+      </c>
+      <c r="D17" s="51">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>-5</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="5"/>
+        <v>30.48</v>
+      </c>
+      <c r="H17" s="58">
+        <f t="shared" si="6"/>
+        <v>152.4</v>
+      </c>
+      <c r="I17" s="59">
+        <f t="shared" si="7"/>
+        <v>1.524E-2</v>
+      </c>
+      <c r="J17" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="9"/>
+        <v>13.5</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="10"/>
+        <v>3.5</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="O17">
+        <v>30.48</v>
+      </c>
+      <c r="P17" s="56">
+        <f t="shared" si="11"/>
+        <v>30.627281955798821</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="12"/>
+        <v>91.44</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="13"/>
+        <v>9.1439999999999994E-3</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>12</v>
+      </c>
+      <c r="V17">
+        <v>12</v>
+      </c>
+      <c r="W17">
+        <v>2</v>
+      </c>
+      <c r="X17">
+        <v>0.45</v>
+      </c>
+      <c r="Y17">
+        <v>30.48</v>
+      </c>
+      <c r="Z17">
+        <v>4.5</v>
+      </c>
+      <c r="AA17">
+        <v>3.5</v>
+      </c>
+      <c r="AB17">
+        <v>1.2192E-2</v>
+      </c>
+      <c r="AC17">
+        <v>5.4863999999999997</v>
+      </c>
+      <c r="AD17">
+        <v>0.30887399999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B18" s="50">
+        <v>14</v>
+      </c>
+      <c r="C18" s="17">
+        <v>0</v>
+      </c>
+      <c r="D18" s="51">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="5"/>
+        <v>30.48</v>
+      </c>
+      <c r="H18" s="58">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="59">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="9"/>
+        <v>14.5</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="10"/>
+        <v>2.5</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>30.48</v>
+      </c>
+      <c r="P18" s="56">
+        <f t="shared" si="11"/>
+        <v>30.887382537210886</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="12"/>
+        <v>38.1</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="13"/>
+        <v>3.81E-3</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>13</v>
+      </c>
+      <c r="V18">
+        <v>13</v>
+      </c>
+      <c r="W18">
+        <v>5</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <v>30.48</v>
+      </c>
+      <c r="Z18">
+        <v>3.5</v>
+      </c>
+      <c r="AA18">
+        <v>2.5</v>
+      </c>
+      <c r="AB18">
+        <v>9.1439999999999994E-3</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>0.30627300000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B19" s="50">
+        <v>15</v>
+      </c>
+      <c r="C19" s="17">
+        <v>0</v>
+      </c>
+      <c r="D19" s="51">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="5"/>
+        <v>30.48</v>
+      </c>
+      <c r="H19" s="58">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="59">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="9"/>
+        <v>15.5</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>30.48</v>
+      </c>
+      <c r="P19" s="56">
+        <f t="shared" si="11"/>
+        <v>30.48</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>14</v>
+      </c>
+      <c r="V19">
+        <v>14</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19">
+        <v>30.48</v>
+      </c>
+      <c r="Z19">
+        <v>2.5</v>
+      </c>
+      <c r="AA19">
+        <v>0</v>
+      </c>
+      <c r="AB19">
+        <v>3.81E-3</v>
+      </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
+      <c r="AD19">
+        <v>0.30887399999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="52">
+        <v>16</v>
+      </c>
+      <c r="C20" s="53">
+        <v>0</v>
+      </c>
+      <c r="D20" s="54">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="5"/>
+        <v>30.48</v>
+      </c>
+      <c r="H20" s="58">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="59">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="L20">
         <f t="shared" si="9"/>
         <v>16.5</v>
       </c>
-      <c r="N8">
-        <f>(C8+C9)/2</f>
-        <v>19.5</v>
-      </c>
-      <c r="O8">
-        <v>30.48</v>
-      </c>
-      <c r="P8" s="56">
-        <f>SQRT((C8-C7)^2+((B8-B7)*12*2.54)^2)</f>
-        <v>30.887382537210886</v>
-      </c>
-      <c r="Q8">
+      <c r="M20">
         <f t="shared" si="10"/>
-        <v>548.64</v>
-      </c>
-      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>30.48</v>
+      </c>
+      <c r="P20" s="56">
         <f t="shared" si="11"/>
-        <v>5.4863999999999996E-2</v>
-      </c>
-      <c r="S8">
-        <f t="shared" si="2"/>
-        <v>3.2918399999999994E-3</v>
-      </c>
-      <c r="U8">
-        <v>3</v>
-      </c>
-      <c r="V8">
-        <v>3</v>
-      </c>
-      <c r="W8">
-        <v>14</v>
-      </c>
-      <c r="X8">
-        <v>0.24</v>
-      </c>
-      <c r="Y8">
-        <v>30.48</v>
-      </c>
-      <c r="Z8">
-        <v>14</v>
-      </c>
-      <c r="AA8">
-        <v>16.5</v>
-      </c>
-      <c r="AB8">
-        <v>4.6482000000000002E-2</v>
-      </c>
-      <c r="AC8">
-        <v>11.15568</v>
-      </c>
-      <c r="AD8">
-        <v>0.30480000000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="2:30">
-      <c r="B9" s="14">
-        <v>5</v>
-      </c>
-      <c r="C9" s="15">
-        <v>20</v>
-      </c>
-      <c r="D9" s="16">
-        <v>0.32</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="1"/>
-        <v>-20</v>
-      </c>
-      <c r="F9">
+        <v>30.48</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="S20">
         <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="4"/>
-        <v>30.48</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="5"/>
-        <v>609.6</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="6"/>
-        <v>6.096E-2</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="0"/>
-        <v>1.9507199999999999E-2</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="7"/>
-        <v>5</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="8"/>
-        <v>5.5</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="9"/>
-        <v>19.5</v>
-      </c>
-      <c r="N9">
-        <f>(C9+C10)/2</f>
-        <v>16</v>
-      </c>
-      <c r="O9">
-        <v>30.48</v>
-      </c>
-      <c r="P9" s="56">
-        <f>SQRT((C9-C8)^2+((B9-B8)*12*2.54)^2)</f>
-        <v>30.496399787515902</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="10"/>
-        <v>541.02</v>
-      </c>
-      <c r="R9">
-        <f t="shared" si="11"/>
-        <v>5.4101999999999997E-2</v>
-      </c>
-      <c r="S9">
-        <f t="shared" si="2"/>
-        <v>1.7312640000000001E-2</v>
-      </c>
-      <c r="U9">
-        <v>4</v>
-      </c>
-      <c r="V9">
-        <v>4</v>
-      </c>
-      <c r="W9">
-        <v>19</v>
-      </c>
-      <c r="X9">
-        <v>0.06</v>
-      </c>
-      <c r="Y9">
-        <v>30.48</v>
-      </c>
-      <c r="Z9">
-        <v>16.5</v>
-      </c>
-      <c r="AA9">
-        <v>19.5</v>
-      </c>
-      <c r="AB9">
-        <v>5.4864000000000003E-2</v>
-      </c>
-      <c r="AC9">
-        <v>3.2918400000000001</v>
-      </c>
-      <c r="AD9">
-        <v>0.30887399999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="2:30">
-      <c r="B10" s="14">
-        <v>6</v>
-      </c>
-      <c r="C10" s="15">
-        <v>12</v>
-      </c>
-      <c r="D10" s="16">
-        <v>0.47</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="1"/>
-        <v>-12</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="4"/>
-        <v>30.48</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="5"/>
-        <v>365.76</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="6"/>
-        <v>3.6575999999999997E-2</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="0"/>
-        <v>1.7190719999999996E-2</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="7"/>
-        <v>6</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="8"/>
-        <v>6.5</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="9"/>
-        <v>16</v>
-      </c>
-      <c r="N10">
-        <f>(C10+C11)/2</f>
-        <v>11</v>
-      </c>
-      <c r="O10">
-        <v>30.48</v>
-      </c>
-      <c r="P10" s="56">
-        <f>SQRT((C10-C9)^2+((B10-B9)*12*2.54)^2)</f>
-        <v>31.512384866905901</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="10"/>
-        <v>411.48</v>
-      </c>
-      <c r="R10">
-        <f t="shared" si="11"/>
-        <v>4.1148000000000004E-2</v>
-      </c>
-      <c r="S10">
-        <f t="shared" si="2"/>
-        <v>1.9339560000000002E-2</v>
-      </c>
-      <c r="U10">
-        <v>5</v>
-      </c>
-      <c r="V10">
-        <v>5</v>
-      </c>
-      <c r="W10">
-        <v>20</v>
-      </c>
-      <c r="X10">
-        <v>0.32</v>
-      </c>
-      <c r="Y10">
-        <v>30.48</v>
-      </c>
-      <c r="Z10">
-        <v>19.5</v>
-      </c>
-      <c r="AA10">
-        <v>16</v>
-      </c>
-      <c r="AB10">
-        <v>5.4101999999999997E-2</v>
-      </c>
-      <c r="AC10">
-        <v>17.312639999999998</v>
-      </c>
-      <c r="AD10">
-        <v>0.30496400000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="2:30">
-      <c r="B11" s="14">
-        <v>7</v>
-      </c>
-      <c r="C11" s="15">
-        <v>10</v>
-      </c>
-      <c r="D11" s="16">
-        <v>0.26</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="1"/>
-        <v>-10</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="4"/>
-        <v>30.48</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="5"/>
-        <v>304.8</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="6"/>
-        <v>3.048E-2</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="0"/>
-        <v>7.9248000000000009E-3</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="7"/>
-        <v>7</v>
-      </c>
-      <c r="L11">
-        <f t="shared" si="8"/>
-        <v>7.5</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="9"/>
-        <v>11</v>
-      </c>
-      <c r="N11">
-        <f>(C11+C12)/2</f>
-        <v>10</v>
-      </c>
-      <c r="O11">
-        <v>30.48</v>
-      </c>
-      <c r="P11" s="56">
-        <f>SQRT((C11-C10)^2+((B11-B10)*12*2.54)^2)</f>
-        <v>30.545546320208452</v>
-      </c>
-      <c r="Q11">
-        <f t="shared" si="10"/>
-        <v>320.04000000000002</v>
-      </c>
-      <c r="R11">
-        <f t="shared" si="11"/>
-        <v>3.2004000000000005E-2</v>
-      </c>
-      <c r="S11">
-        <f t="shared" si="2"/>
-        <v>8.3210400000000018E-3</v>
-      </c>
-      <c r="U11">
-        <v>6</v>
-      </c>
-      <c r="V11">
-        <v>6</v>
-      </c>
-      <c r="W11">
-        <v>12</v>
-      </c>
-      <c r="X11">
-        <v>0.47</v>
-      </c>
-      <c r="Y11">
-        <v>30.48</v>
-      </c>
-      <c r="Z11">
-        <v>16</v>
-      </c>
-      <c r="AA11">
-        <v>11</v>
-      </c>
-      <c r="AB11">
-        <v>4.1147999999999997E-2</v>
-      </c>
-      <c r="AC11">
-        <v>19.339559999999999</v>
-      </c>
-      <c r="AD11">
-        <v>0.31512400000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="2:30">
-      <c r="B12" s="14">
-        <v>8</v>
-      </c>
-      <c r="C12" s="15">
-        <v>10</v>
-      </c>
-      <c r="D12" s="16">
-        <v>0.33</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="1"/>
-        <v>-10</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="4"/>
-        <v>30.48</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="5"/>
-        <v>304.8</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="6"/>
-        <v>3.048E-2</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="0"/>
-        <v>1.00584E-2</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="8"/>
-        <v>8.5</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="9"/>
-        <v>10</v>
-      </c>
-      <c r="N12">
-        <f>(C12+C13)/2</f>
-        <v>7</v>
-      </c>
-      <c r="O12">
-        <v>30.48</v>
-      </c>
-      <c r="P12" s="56">
-        <f>SQRT((C12-C11)^2+((B12-B11)*12*2.54)^2)</f>
-        <v>30.48</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" si="10"/>
-        <v>259.08</v>
-      </c>
-      <c r="R12">
-        <f t="shared" si="11"/>
-        <v>2.5907999999999997E-2</v>
-      </c>
-      <c r="S12">
-        <f t="shared" si="2"/>
-        <v>8.549639999999999E-3</v>
-      </c>
-      <c r="U12">
-        <v>7</v>
-      </c>
-      <c r="V12">
-        <v>7</v>
-      </c>
-      <c r="W12">
-        <v>10</v>
-      </c>
-      <c r="X12">
-        <v>0.26</v>
-      </c>
-      <c r="Y12">
-        <v>30.48</v>
-      </c>
-      <c r="Z12">
-        <v>11</v>
-      </c>
-      <c r="AA12">
-        <v>10</v>
-      </c>
-      <c r="AB12">
-        <v>3.2003999999999998E-2</v>
-      </c>
-      <c r="AC12">
-        <v>8.32104</v>
-      </c>
-      <c r="AD12">
-        <v>0.30545499999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="2:30">
-      <c r="B13" s="14">
-        <v>9</v>
-      </c>
-      <c r="C13" s="15">
-        <v>4</v>
-      </c>
-      <c r="D13" s="16">
-        <v>0.2</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="1"/>
-        <v>-4</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="4"/>
-        <v>30.48</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="5"/>
-        <v>121.92</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="6"/>
-        <v>1.2192E-2</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="0"/>
-        <v>2.4384000000000003E-3</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="7"/>
-        <v>9</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="8"/>
-        <v>9.5</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="9"/>
-        <v>7</v>
-      </c>
-      <c r="N13">
-        <f>(C13+C14)/2</f>
-        <v>6</v>
-      </c>
-      <c r="O13">
-        <v>30.48</v>
-      </c>
-      <c r="P13" s="56">
-        <f>SQRT((C13-C12)^2+((B13-B12)*12*2.54)^2)</f>
-        <v>31.064938435477384</v>
-      </c>
-      <c r="Q13">
-        <f t="shared" si="10"/>
-        <v>198.12</v>
-      </c>
-      <c r="R13">
-        <f t="shared" si="11"/>
-        <v>1.9812E-2</v>
-      </c>
-      <c r="S13">
-        <f t="shared" si="2"/>
-        <v>3.9624000000000005E-3</v>
-      </c>
-      <c r="U13">
-        <v>8</v>
-      </c>
-      <c r="V13">
-        <v>8</v>
-      </c>
-      <c r="W13">
-        <v>10</v>
-      </c>
-      <c r="X13">
-        <v>0.33</v>
-      </c>
-      <c r="Y13">
-        <v>30.48</v>
-      </c>
-      <c r="Z13">
-        <v>10</v>
-      </c>
-      <c r="AA13">
-        <v>7</v>
-      </c>
-      <c r="AB13">
-        <v>2.5908E-2</v>
-      </c>
-      <c r="AC13">
-        <v>8.5496400000000001</v>
-      </c>
-      <c r="AD13">
-        <v>0.30480000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="2:30">
-      <c r="B14" s="14">
-        <v>10</v>
-      </c>
-      <c r="C14" s="15">
-        <v>8</v>
-      </c>
-      <c r="D14" s="16">
-        <v>0.13</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="1"/>
-        <v>-8</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="4"/>
-        <v>30.48</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="5"/>
-        <v>243.84</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="6"/>
-        <v>2.4383999999999999E-2</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="0"/>
-        <v>3.1699200000000001E-3</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="7"/>
-        <v>10</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="8"/>
-        <v>10.5</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="9"/>
-        <v>6</v>
-      </c>
-      <c r="N14">
-        <f>(C14+C15)/2</f>
-        <v>7.5</v>
-      </c>
-      <c r="O14">
-        <v>30.48</v>
-      </c>
-      <c r="P14" s="56">
-        <f>SQRT((C14-C13)^2+((B14-B13)*12*2.54)^2)</f>
-        <v>30.741346749939243</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" si="10"/>
-        <v>205.74</v>
-      </c>
-      <c r="R14">
-        <f t="shared" si="11"/>
-        <v>2.0574000000000002E-2</v>
-      </c>
-      <c r="S14">
-        <f t="shared" si="2"/>
-        <v>2.6746200000000004E-3</v>
-      </c>
-      <c r="U14">
-        <v>9</v>
-      </c>
-      <c r="V14">
-        <v>9</v>
-      </c>
-      <c r="W14">
-        <v>4</v>
-      </c>
-      <c r="X14">
-        <v>0.2</v>
-      </c>
-      <c r="Y14">
-        <v>30.48</v>
-      </c>
-      <c r="Z14">
-        <v>7</v>
-      </c>
-      <c r="AA14">
-        <v>6</v>
-      </c>
-      <c r="AB14">
-        <v>1.9812E-2</v>
-      </c>
-      <c r="AC14">
-        <v>3.9624000000000001</v>
-      </c>
-      <c r="AD14">
-        <v>0.31064900000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="2:30">
-      <c r="B15" s="14">
-        <v>11</v>
-      </c>
-      <c r="C15" s="15">
-        <v>7</v>
-      </c>
-      <c r="D15" s="16">
-        <v>0.02</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="1"/>
-        <v>-7</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="4"/>
-        <v>30.48</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="5"/>
-        <v>213.36</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="6"/>
-        <v>2.1336000000000001E-2</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="0"/>
-        <v>4.2672000000000001E-4</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="7"/>
-        <v>11</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="8"/>
-        <v>11.5</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="9"/>
-        <v>7.5</v>
-      </c>
-      <c r="N15">
-        <f>(C15+C16)/2</f>
-        <v>4.5</v>
-      </c>
-      <c r="O15">
-        <v>30.48</v>
-      </c>
-      <c r="P15" s="56">
-        <f>SQRT((C15-C14)^2+((B15-B14)*12*2.54)^2)</f>
-        <v>30.496399787515902</v>
-      </c>
-      <c r="Q15">
-        <f t="shared" si="10"/>
-        <v>182.88</v>
-      </c>
-      <c r="R15">
-        <f t="shared" si="11"/>
-        <v>1.8287999999999999E-2</v>
-      </c>
-      <c r="S15">
-        <f t="shared" si="2"/>
-        <v>3.6575999999999997E-4</v>
-      </c>
-      <c r="U15">
-        <v>10</v>
-      </c>
-      <c r="V15">
-        <v>10</v>
-      </c>
-      <c r="W15">
-        <v>8</v>
-      </c>
-      <c r="X15">
-        <v>0.13</v>
-      </c>
-      <c r="Y15">
-        <v>30.48</v>
-      </c>
-      <c r="Z15">
-        <v>6</v>
-      </c>
-      <c r="AA15">
-        <v>7.5</v>
-      </c>
-      <c r="AB15">
-        <v>2.0573999999999999E-2</v>
-      </c>
-      <c r="AC15">
-        <v>2.67462</v>
-      </c>
-      <c r="AD15">
-        <v>0.30741299999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="2:30">
-      <c r="B16" s="14">
-        <v>12</v>
-      </c>
-      <c r="C16" s="15">
-        <v>2</v>
-      </c>
-      <c r="D16" s="16">
-        <v>0.45</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="1"/>
-        <v>-2</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="4"/>
-        <v>30.48</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="5"/>
-        <v>60.96</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="6"/>
-        <v>6.0959999999999999E-3</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="0"/>
-        <v>2.7431999999999999E-3</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="7"/>
-        <v>12</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="8"/>
-        <v>12.5</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="9"/>
-        <v>4.5</v>
-      </c>
-      <c r="N16">
-        <f>(C16+C17)/2</f>
-        <v>3.5</v>
-      </c>
-      <c r="O16">
-        <v>30.48</v>
-      </c>
-      <c r="P16" s="56">
-        <f>SQRT((C16-C15)^2+((B16-B15)*12*2.54)^2)</f>
-        <v>30.887382537210886</v>
-      </c>
-      <c r="Q16">
-        <f t="shared" si="10"/>
-        <v>121.92</v>
-      </c>
-      <c r="R16">
-        <f t="shared" si="11"/>
-        <v>1.2192E-2</v>
-      </c>
-      <c r="S16">
-        <f t="shared" si="2"/>
-        <v>5.4863999999999998E-3</v>
-      </c>
-      <c r="U16">
-        <v>11</v>
-      </c>
-      <c r="V16">
-        <v>11</v>
-      </c>
-      <c r="W16">
-        <v>7</v>
-      </c>
-      <c r="X16">
-        <v>0.02</v>
-      </c>
-      <c r="Y16">
-        <v>30.48</v>
-      </c>
-      <c r="Z16">
-        <v>7.5</v>
-      </c>
-      <c r="AA16">
-        <v>4.5</v>
-      </c>
-      <c r="AB16">
-        <v>1.8287999999999999E-2</v>
-      </c>
-      <c r="AC16">
-        <v>0.36575999999999997</v>
-      </c>
-      <c r="AD16">
-        <v>0.30496400000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="2:30">
-      <c r="B17" s="50">
-        <v>13</v>
-      </c>
-      <c r="C17" s="17">
-        <v>5</v>
-      </c>
-      <c r="D17" s="51">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="1"/>
-        <v>-5</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="4"/>
-        <v>30.48</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="5"/>
-        <v>152.4</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="6"/>
-        <v>1.524E-2</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="7"/>
-        <v>13</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="8"/>
-        <v>13.5</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="9"/>
-        <v>3.5</v>
-      </c>
-      <c r="N17">
-        <f>(C17+C18)/2</f>
-        <v>2.5</v>
-      </c>
-      <c r="O17">
-        <v>30.48</v>
-      </c>
-      <c r="P17" s="56">
-        <f>SQRT((C17-C16)^2+((B17-B16)*12*2.54)^2)</f>
-        <v>30.627281955798821</v>
-      </c>
-      <c r="Q17">
-        <f t="shared" si="10"/>
-        <v>91.44</v>
-      </c>
-      <c r="R17">
-        <f t="shared" si="11"/>
-        <v>9.1439999999999994E-3</v>
-      </c>
-      <c r="S17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="U17">
-        <v>12</v>
-      </c>
-      <c r="V17">
-        <v>12</v>
-      </c>
-      <c r="W17">
-        <v>2</v>
-      </c>
-      <c r="X17">
-        <v>0.45</v>
-      </c>
-      <c r="Y17">
-        <v>30.48</v>
-      </c>
-      <c r="Z17">
-        <v>4.5</v>
-      </c>
-      <c r="AA17">
-        <v>3.5</v>
-      </c>
-      <c r="AB17">
-        <v>1.2192E-2</v>
-      </c>
-      <c r="AC17">
-        <v>5.4863999999999997</v>
-      </c>
-      <c r="AD17">
-        <v>0.30887399999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="2:30">
-      <c r="B18" s="50">
-        <v>14</v>
-      </c>
-      <c r="C18" s="17">
-        <v>0</v>
-      </c>
-      <c r="D18" s="51">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="4"/>
-        <v>30.48</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="7"/>
-        <v>14</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="8"/>
-        <v>14.5</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="9"/>
-        <v>2.5</v>
-      </c>
-      <c r="N18">
-        <f>(C18+C19)/2</f>
-        <v>0</v>
-      </c>
-      <c r="O18">
-        <v>30.48</v>
-      </c>
-      <c r="P18" s="56">
-        <f>SQRT((C18-C17)^2+((B18-B17)*12*2.54)^2)</f>
-        <v>30.887382537210886</v>
-      </c>
-      <c r="Q18">
-        <f t="shared" si="10"/>
-        <v>38.1</v>
-      </c>
-      <c r="R18">
-        <f t="shared" si="11"/>
-        <v>3.81E-3</v>
-      </c>
-      <c r="S18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="U18">
-        <v>13</v>
-      </c>
-      <c r="V18">
-        <v>13</v>
-      </c>
-      <c r="W18">
-        <v>5</v>
-      </c>
-      <c r="X18">
-        <v>0</v>
-      </c>
-      <c r="Y18">
-        <v>30.48</v>
-      </c>
-      <c r="Z18">
-        <v>3.5</v>
-      </c>
-      <c r="AA18">
-        <v>2.5</v>
-      </c>
-      <c r="AB18">
-        <v>9.1439999999999994E-3</v>
-      </c>
-      <c r="AC18">
-        <v>0</v>
-      </c>
-      <c r="AD18">
-        <v>0.30627300000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="2:30">
-      <c r="B19" s="50">
-        <v>15</v>
-      </c>
-      <c r="C19" s="17">
-        <v>0</v>
-      </c>
-      <c r="D19" s="51">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="4"/>
-        <v>30.48</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="7"/>
-        <v>15</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="8"/>
-        <v>15.5</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <f>(C19+C20)/2</f>
-        <v>0</v>
-      </c>
-      <c r="O19">
-        <v>30.48</v>
-      </c>
-      <c r="P19" s="56">
-        <f>SQRT((C19-C18)^2+((B19-B18)*12*2.54)^2)</f>
-        <v>30.48</v>
-      </c>
-      <c r="Q19">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="R19">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="S19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="U19">
-        <v>14</v>
-      </c>
-      <c r="V19">
-        <v>14</v>
-      </c>
-      <c r="W19">
-        <v>0</v>
-      </c>
-      <c r="X19">
-        <v>0</v>
-      </c>
-      <c r="Y19">
-        <v>30.48</v>
-      </c>
-      <c r="Z19">
-        <v>2.5</v>
-      </c>
-      <c r="AA19">
-        <v>0</v>
-      </c>
-      <c r="AB19">
-        <v>3.81E-3</v>
-      </c>
-      <c r="AC19">
-        <v>0</v>
-      </c>
-      <c r="AD19">
-        <v>0.30887399999999998</v>
-      </c>
-    </row>
-    <row r="20" spans="2:30" ht="15.75" thickBot="1">
-      <c r="B20" s="52">
-        <v>16</v>
-      </c>
-      <c r="C20" s="53">
-        <v>0</v>
-      </c>
-      <c r="D20" s="54">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="4"/>
-        <v>30.48</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="7"/>
-        <v>16</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="8"/>
-        <v>16.5</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20">
-        <v>30.48</v>
-      </c>
-      <c r="P20" s="56">
-        <f>SQRT((C20-C19)^2+((B20-B19)*12*2.54)^2)</f>
-        <v>30.48</v>
-      </c>
-      <c r="Q20">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="R20">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="S20">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U20">
@@ -5273,7 +5386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:30">
+    <row r="21" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C21">
         <f>AVERAGE(C6:C16)</f>
         <v>10.909090909090908</v>
@@ -5329,7 +5442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:30">
+    <row r="22" spans="2:30" x14ac:dyDescent="0.25">
       <c r="H22" t="s">
         <v>17</v>
       </c>
@@ -5356,12 +5469,12 @@
         <v>97.330259999999996</v>
       </c>
     </row>
-    <row r="23" spans="2:30">
+    <row r="23" spans="2:30" x14ac:dyDescent="0.25">
       <c r="L23" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="2:30">
+    <row r="24" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B24" s="30"/>
       <c r="C24" s="30" t="s">
         <v>37</v>
@@ -5370,7 +5483,7 @@
       <c r="E24" s="30"/>
       <c r="U24" s="4"/>
     </row>
-    <row r="25" spans="2:30">
+    <row r="25" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B25" s="30"/>
       <c r="C25" s="30" t="s">
         <v>38</v>
@@ -5378,7 +5491,7 @@
       <c r="D25" s="30"/>
       <c r="E25" s="30"/>
     </row>
-    <row r="26" spans="2:30">
+    <row r="26" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B26" s="30" t="s">
         <v>30</v>
       </c>
@@ -5393,7 +5506,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="2:30">
+    <row r="27" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B27" s="30"/>
       <c r="C27" s="30" t="s">
         <v>24</v>
@@ -5406,7 +5519,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="2:30">
+    <row r="28" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B28" s="30"/>
       <c r="C28" s="30" t="s">
         <v>26</v>
@@ -5419,7 +5532,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="2:30">
+    <row r="29" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B29" s="30"/>
       <c r="C29" s="30" t="s">
         <v>23</v>
@@ -5431,7 +5544,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="2:30">
+    <row r="30" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B30" s="30"/>
       <c r="C30" s="30" t="s">
         <v>22</v>
@@ -5441,7 +5554,7 @@
       </c>
       <c r="E30" s="30"/>
     </row>
-    <row r="31" spans="2:30">
+    <row r="31" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B31" s="30"/>
       <c r="C31" s="30"/>
       <c r="D31" s="30" t="s">
@@ -5449,7 +5562,7 @@
       </c>
       <c r="E31" s="30"/>
     </row>
-    <row r="32" spans="2:30">
+    <row r="32" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B32" s="30"/>
       <c r="C32" s="30" t="s">
         <v>36</v>
@@ -5462,7 +5575,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="2:5">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="30"/>
       <c r="C33" s="30" t="s">
         <v>39</v>
@@ -5475,7 +5588,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="2:5">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="30"/>
       <c r="C34" s="30"/>
       <c r="D34" s="46">

</xml_diff>